<commit_message>
added Kansas City, MO
</commit_message>
<xml_diff>
--- a/Athens/Athens.xlsx
+++ b/Athens/Athens.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -43,9 +43,6 @@
     <t xml:space="preserve">Independent Agencies*</t>
   </si>
   <si>
-    <t xml:space="preserve">7056784</t>
-  </si>
-  <si>
     <t xml:space="preserve">Information Technology</t>
   </si>
   <si>
@@ -55,7 +52,7 @@
     <t xml:space="preserve">Planning</t>
   </si>
   <si>
-    <t xml:space="preserve">Police</t>
+    <t xml:space="preserve">Police + Sheriff</t>
   </si>
   <si>
     <t xml:space="preserve">Solid Waste Services</t>
@@ -73,7 +70,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -156,8 +153,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -181,18 +178,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.29081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,8 +242,8 @@
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
+      <c r="C5" s="2" t="n">
+        <v>7056784</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,7 +251,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>8095600</v>
@@ -266,7 +262,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>3606600</v>
@@ -277,7 +273,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1752100</v>
@@ -288,11 +284,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="n">
-        <f aca="false">25370400</f>
-        <v>25370400</v>
+        <f aca="false">25370400+17854300</f>
+        <v>43224700</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,7 +296,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>6500800</v>
@@ -311,7 +307,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>6225200</v>
@@ -322,10 +318,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>7877300</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="2" t="n">
+        <v>5000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>